<commit_message>
Back probado casi que por completo :))))
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -24,24 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ángulo del contad</t>
   </si>
   <si>
-    <t>Tasa con 15kV</t>
-  </si>
-  <si>
-    <t>Tasa con 25kV</t>
+    <t>Tasa con 35kV</t>
   </si>
   <si>
     <t>2*theta/°</t>
   </si>
   <si>
-    <t>R(15kV)/Imp/s</t>
-  </si>
-  <si>
-    <t>R(25kV)/Imp/s</t>
+    <t>R(35kV)/Imp/s</t>
   </si>
 </sst>
 </file>
@@ -359,56 +353,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>13080</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>13978</v>
-      </c>
-      <c r="C4">
-        <v>13614</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5">
+        <v>13031</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>12485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>30</v>
       </c>
-      <c r="B5">
-        <v>12991</v>
-      </c>
-      <c r="C5">
-        <v>12970</v>
+      <c r="B7">
+        <v>13283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>12750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>11838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglado socket y problema con inicios consecutivo. Falta arreglar ángulos y el tiempo en front
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -24,15 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Ángulo del contad</t>
   </si>
   <si>
+    <t>Tasa con 30kV</t>
+  </si>
+  <si>
     <t>Tasa con 35kV</t>
   </si>
   <si>
     <t>2*theta/°</t>
+  </si>
+  <si>
+    <t>R(30kV)/Imp/s</t>
   </si>
   <si>
     <t>R(35kV)/Imp/s</t>
@@ -353,76 +359,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B4">
-        <v>13080</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>13031</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>12485</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>13283</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>40</v>
-      </c>
-      <c r="B8">
-        <v>12750</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>50</v>
-      </c>
-      <c r="B9">
-        <v>11838</v>
+        <v>12571</v>
+      </c>
+      <c r="C4">
+        <v>12866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se intentó arreglar el bug pero no se pudo, toca seguirlo mirando. Es el de Excel
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ángulo del contad</t>
   </si>
@@ -32,16 +32,10 @@
     <t>Tasa con 30kV</t>
   </si>
   <si>
-    <t>Tasa con 35kV</t>
-  </si>
-  <si>
     <t>2*theta/°</t>
   </si>
   <si>
     <t>R(30kV)/Imp/s</t>
-  </si>
-  <si>
-    <t>R(35kV)/Imp/s</t>
   </si>
 </sst>
 </file>
@@ -359,45 +353,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>12571</v>
-      </c>
-      <c r="C4">
-        <v>12866</v>
+        <v>13347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>13299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>12012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>3535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>110</v>
+      </c>
+      <c r="B9">
+        <v>1084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregidos algunos scripts de Autoit3 para evitar bugs
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="4">
   <si>
     <t>Ángulo del contad</t>
   </si>
@@ -353,76 +353,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection sqref="A1:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B4">
-        <v>13347</v>
+        <v>13183</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B5">
-        <v>13299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>12012</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>70</v>
-      </c>
-      <c r="B7">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>90</v>
-      </c>
-      <c r="B8">
-        <v>3535</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>110</v>
-      </c>
-      <c r="B9">
-        <v>1084</v>
+        <v>12352</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>